<commit_message>
début revenus... à compléter
</commit_message>
<xml_diff>
--- a/includes/pour_calculs/calculs_MS.xlsx
+++ b/includes/pour_calculs/calculs_MS.xlsx
@@ -1039,7 +1039,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1080,7 +1080,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1096,11 +1096,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1109,10 +1113,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1196,23 +1196,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1237,7 +1221,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1248,10 +1232,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0944113416889254"/>
-          <c:y val="0.0815165876777251"/>
-          <c:w val="0.88550441750565"/>
-          <c:h val="0.777369668246446"/>
+          <c:x val="0.0944161915035701"/>
+          <c:y val="0.0815262471856855"/>
+          <c:w val="0.885447167000565"/>
+          <c:h val="0.777224789667022"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1295,451 +1279,451 @@
               <c:strCache>
                 <c:ptCount val="149"/>
                 <c:pt idx="0">
-                  <c:v>1861</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1862</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1863</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1864</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1865</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1866</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1867</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1868</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1869</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1870</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1871</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1872</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1873</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1874</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1876</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1877</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1878</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1879</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1880</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1881</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1882</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1883</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1884</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1885</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1886</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1887</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1888</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1889</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1890</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1891</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1892</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1893</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1894</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1895</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1896</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1897</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1898</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1899</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1900</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1901</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1902</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1903</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1904</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1905</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1906</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1907</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1908</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1909</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1910</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1911</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1912</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1913</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1914</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1915</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1916</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1917</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1918</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1919</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1920</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1921</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1922</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1923</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1924</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1925</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1926</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1927</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1928</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1929</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1930</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1931</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1932</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1933</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1934</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1935</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1936</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1937</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1938</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1939</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1940</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1941</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1942</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1943</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1944</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1945</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1946</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1947</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1948</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1949</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1950</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1951</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1952</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1953</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1954</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1955</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1956</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1957</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1958</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1959</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1960</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1961</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1962</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1963</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1964</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1965</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1966</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1967</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1968</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1969</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1970</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>1971</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>1972</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>1973</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1974</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1975</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>1976</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>1977</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>1978</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>1979</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>1980</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>1981</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>1982</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>1983</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>1984</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>1985</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>1986</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>1987</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>1988</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>1989</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>1990</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>1991</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>1992</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>1993</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>1994</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>1995</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>1996</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>1997</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>1998</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>1999</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>2000</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>2001</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>2002</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>2003</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>2004</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>2005</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>2006</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>2007</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>2008</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>2009</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1751,451 +1735,451 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="149"/>
                 <c:pt idx="0">
-                  <c:v>11.65258359111</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.472839782855</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54.6636643366743</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110.1100842856</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.9851019683319</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54.576896615505</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.8432271269936</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>58.2688631512597</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>58.429383435423</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>65.221925986331</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>77.406448140945</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64.92153715047</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>32.6391244465275</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22.0951449965885</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>26.26695559035</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>51.36649093224</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>48.5573859593831</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>26.3474673316231</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.7210634829136</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>21.0336924075983</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>19.041026811089</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>17.2697685030807</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.9314691661786</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>19.97585758476</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>20.92708889832</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>16.88435581569</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>15.93312450213</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>20.92708889832</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>22.35393586866</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>20.68928106993</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>15.93312450213</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>13.31723838984</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>15.21970101696</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>20.7441597995585</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>34.9292138339232</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>30.3062296500216</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>20.2897639182348</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>23.3717533741692</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>33.1313866512948</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>30.5630621046828</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>24.6559156474752</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>20.546596372896</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>23.2137026328392</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>20.45147324154</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>14.74408536018</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>17.35997147247</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>17.12216364408</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>16.5106577996486</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>16.6465479873</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>13.9881961913689</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>13.9881961913689</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>16.3841393490765</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>20.5379488155</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>17.2767075174</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>13.5148012224</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>21.597868864</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>26.0814347196</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>28.184369301</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>24.9201673923</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>32.8589803551</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>20.7286722085</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>20.5930204634</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>16.8376790006</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>17.9317533395</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>20.5476673416</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>22.7760202532</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>16.050585655</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>14.6413135557</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>15.8927078767</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>15.2821999358</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>9.1520411515</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>13.6569748923</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>11.0852126048</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>16.01304168</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>15.1518258009</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>16.8672636529</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>17.6220262726</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>17.1953336333</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>15.744655893</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>15.5936647524</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>16.6015595784</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>15.6549365196</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>14.877711876</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>14.744698936</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>12.506648952</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>12.290395656</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>18.236932222</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>17.7218074313</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>16.0120548098</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>15.2282867877</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>14.1093690642</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>13.8122138655</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>15.4650069135</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>15.3904767597</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>15.4525852212</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>15.2289947598</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>14.466444447</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>15.4264117072</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>15.2925406192</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>13.749032719</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>12.89796444</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>12.758944464</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>12.60833949</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>12.43456452</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>12.226034556</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>11.89393128</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>11.557966338</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>11.094566418</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>10.526901516</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>9.939928284</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>11.8506806208</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>12.7213575816</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>15.8881596923</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>50.4072273534</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>45.9844398299</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>48.248513152</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>49.2449946096</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>46.1320358895706</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>93.4092915977962</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>95.890748907767</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>84.7999385038504</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>73.298289015544</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>63.6502846385542</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>59.426129547642</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>54.9501832713755</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>28.2460666970803</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>34.8151236598398</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>27.0643806153246</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>31.5336747503395</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>38.9446542440788</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>31.5085627801204</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>29.5440792705217</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>25.1975327776152</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>22.8974315186397</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>23.9547730498615</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>28.2610292917196</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>25.5206632055296</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>16.7360728296043</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>23.1407357801837</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>35.5013251162625</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>29.611061913725</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>29.8411018875186</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>33.6155029943734</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>43.458222895712</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>59.8914028574578</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>69.3244629789807</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>74.9010606278554</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>96.909957764609</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>61.6712648</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2240,451 +2224,451 @@
               <c:strCache>
                 <c:ptCount val="149"/>
                 <c:pt idx="0">
-                  <c:v>1861</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1862</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1863</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1864</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1865</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1866</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1867</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1868</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1869</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1870</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1871</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1872</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1873</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1874</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1876</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1877</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1878</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1879</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1880</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1881</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1882</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1883</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1884</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1885</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1886</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1887</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1888</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1889</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1890</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1891</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1892</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1893</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1894</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1895</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1896</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1897</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1898</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1899</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1900</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1901</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1902</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1903</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1904</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1905</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1906</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1907</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1908</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1909</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1910</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1911</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1912</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1913</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1914</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1915</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1916</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1917</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1918</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1919</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1920</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1921</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1922</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1923</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1924</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1925</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1926</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1927</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1928</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1929</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1930</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1931</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1932</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1933</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1934</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1935</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1936</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1937</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1938</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1939</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1940</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1941</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1942</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1943</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1944</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1945</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1946</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1947</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1948</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1949</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1950</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1951</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1952</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1953</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1954</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1955</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1956</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1957</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1958</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1959</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1960</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1961</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1962</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1963</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1964</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1965</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1966</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1967</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1968</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1969</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1970</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>1971</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>1972</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>1973</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1974</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1975</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>1976</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>1977</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>1978</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>1979</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>1980</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>1981</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>1982</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>1983</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>1984</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>1985</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>1986</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>1987</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>1988</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>1989</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>1990</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>1991</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>1992</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>1993</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>1994</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>1995</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>1996</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>1997</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>1998</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>1999</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>2000</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>2001</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>2002</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>2003</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>2004</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>2005</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>2006</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>2007</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>2008</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>2009</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2696,451 +2680,451 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="149"/>
                 <c:pt idx="0">
-                  <c:v>0.49</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.05</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.15</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.06</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.59</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.74</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.41</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.63</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.64</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.86</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.34</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.64</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.83</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.17</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.35</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.56</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.42</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.19</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.86</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.95</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.86</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.78</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.84</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.88</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.71</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.67</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.88</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.94</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.87</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.67</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.56</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.64</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.84</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.36</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.18</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.79</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.91</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.29</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.19</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.96</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.8</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.94</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.86</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.62</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.73</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.72</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.72</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.7</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.61</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.61</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.74</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.95</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.81</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.64</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.56</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.98</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.01</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>3.07</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.73</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.61</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.34</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.43</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.68</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.88</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.3</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.17</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1.27</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1.19</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.65</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.87</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.67</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.97</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1.09</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1.18</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1.13</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1.02</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1.02</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.14</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.19</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.2</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.21</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.05</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.12</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.99</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1.78</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1.71</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1.71</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1.71</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1.93</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1.93</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.93</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.93</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2.08</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2.08</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.8</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1.8</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1.8</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1.8</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1.8</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1.8</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1.8</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1.8</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1.8</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1.8</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>2.24</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>2.48</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>3.29</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>11.58</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>11.53</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>12.8</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>13.92</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>14.02</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>31.61</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>36.83</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>35.93</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>32.97</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>29.55</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>28.78</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>27.56</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>14.43</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>18.4350394</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>14.9238417</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>18.2261133</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>23.7258203</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>20.0033852</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>19.3208366</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>16.9716342</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>15.8173152</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>17.0166797</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>20.6684884</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>19.0925875</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>12.7156615</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>17.9700778</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>28.4954492</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>24.4438911</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>25.0232558</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>28.8307031</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>38.265</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>54.5210895</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>65.1440625</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>72.3890784</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>97.2559728</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>61.6712648</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3155,11 +3139,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="86082337"/>
-        <c:axId val="55660718"/>
+        <c:axId val="86493214"/>
+        <c:axId val="11215554"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86082337"/>
+        <c:axId val="86493214"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3196,14 +3180,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55660718"/>
+        <c:crossAx val="11215554"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55660718"/>
+        <c:axId val="11215554"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3250,7 +3234,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86082337"/>
+        <c:crossAx val="86493214"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3294,9 +3278,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>666360</xdr:colOff>
+      <xdr:colOff>666000</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3305,7 +3289,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5112720" y="1847880"/>
-        <a:ext cx="7008120" cy="3038040"/>
+        <a:ext cx="7007760" cy="3037680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -10662,7 +10646,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="bottomRight" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10671,7 +10655,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="36.42"/>
@@ -10722,7 +10706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
@@ -10752,7 +10736,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -10781,7 +10765,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -10810,7 +10794,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="11" t="n">
@@ -10831,7 +10815,7 @@
       <c r="H7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="15" t="s">
         <v>34</v>
       </c>
       <c r="J7" s="13" t="s">
@@ -10839,7 +10823,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -10868,7 +10852,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -10897,7 +10881,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -10918,7 +10902,7 @@
       <c r="H10" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="15" t="s">
         <v>48</v>
       </c>
       <c r="J10" s="13" t="n">
@@ -10926,7 +10910,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -10947,7 +10931,7 @@
       <c r="H11" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="15" t="s">
         <v>51</v>
       </c>
       <c r="J11" s="13" t="s">
@@ -10955,7 +10939,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="14" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="11"/>
@@ -10964,11 +10948,11 @@
       <c r="F12" s="11"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="14"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="14" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -10997,7 +10981,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="14" t="s">
         <v>61</v>
       </c>
       <c r="C14" s="11" t="n">
@@ -11018,7 +11002,7 @@
       <c r="H14" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="I14" s="14" t="n">
+      <c r="I14" s="15" t="n">
         <v>1</v>
       </c>
       <c r="J14" s="13" t="n">
@@ -11026,7 +11010,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="14" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="11" t="n">
@@ -11047,7 +11031,7 @@
       <c r="H15" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="I15" s="14" t="n">
+      <c r="I15" s="15" t="n">
         <v>100</v>
       </c>
       <c r="J15" s="13" t="n">
@@ -11055,7 +11039,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C16" s="11" t="n">
@@ -11070,13 +11054,13 @@
       <c r="F16" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="14" t="n">
+      <c r="G16" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="H16" s="14" t="n">
+      <c r="H16" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="I16" s="14" t="n">
+      <c r="I16" s="15" t="n">
         <v>0.3</v>
       </c>
       <c r="J16" s="13" t="n">
@@ -11084,7 +11068,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="14" t="s">
         <v>64</v>
       </c>
       <c r="C17" s="11" t="n">
@@ -11105,36 +11089,36 @@
       <c r="H17" s="12" t="n">
         <v>0.2</v>
       </c>
-      <c r="I17" s="14" t="n">
+      <c r="I17" s="15" t="n">
         <v>0.6</v>
       </c>
       <c r="J17" s="13" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="15" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="15" t="s">
         <v>72</v>
       </c>
       <c r="J18" s="13" t="s">
@@ -11142,7 +11126,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="14" t="s">
         <v>74</v>
       </c>
       <c r="C19" s="11" t="n">
@@ -11167,7 +11151,7 @@
         <f aca="false">100/60</f>
         <v>1.66666666666667</v>
       </c>
-      <c r="I19" s="14" t="n">
+      <c r="I19" s="15" t="n">
         <v>3</v>
       </c>
       <c r="J19" s="13" t="n">
@@ -11175,7 +11159,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="14" t="s">
         <v>75</v>
       </c>
       <c r="C20" s="19" t="s">
@@ -11204,7 +11188,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C21" s="19"/>
@@ -11286,7 +11270,7 @@
   <dimension ref="A3:D692"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D24 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22348,7 +22332,7 @@
   <dimension ref="A3:D692"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G620" activeCellId="1" sqref="D24 G620"/>
+      <selection pane="topLeft" activeCell="G620" activeCellId="0" sqref="G620"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33410,7 +33394,7 @@
   <dimension ref="A1:F711"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D24 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -41498,8 +41482,8 @@
   </sheetPr>
   <dimension ref="A1:C157"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A114" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E146" activeCellId="1" sqref="D24 E146"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -41551,7 +41535,7 @@
       <c r="B5" s="38" t="n">
         <v>0.49</v>
       </c>
-      <c r="C5" s="39" t="n">
+      <c r="C5" s="31" t="n">
         <v>11.65258359111</v>
       </c>
     </row>
@@ -41562,7 +41546,7 @@
       <c r="B6" s="38" t="n">
         <v>1.05</v>
       </c>
-      <c r="C6" s="39" t="n">
+      <c r="C6" s="31" t="n">
         <v>22.472839782855</v>
       </c>
     </row>
@@ -41573,7 +41557,7 @@
       <c r="B7" s="38" t="n">
         <v>3.15</v>
       </c>
-      <c r="C7" s="39" t="n">
+      <c r="C7" s="31" t="n">
         <v>54.6636643366743</v>
       </c>
     </row>
@@ -41584,7 +41568,7 @@
       <c r="B8" s="38" t="n">
         <v>8.06</v>
       </c>
-      <c r="C8" s="39" t="n">
+      <c r="C8" s="31" t="n">
         <v>110.1100842856</v>
       </c>
     </row>
@@ -41595,7 +41579,7 @@
       <c r="B9" s="38" t="n">
         <v>6.59</v>
       </c>
-      <c r="C9" s="39" t="n">
+      <c r="C9" s="31" t="n">
         <v>91.9851019683319</v>
       </c>
     </row>
@@ -41606,7 +41590,7 @@
       <c r="B10" s="38" t="n">
         <v>3.74</v>
       </c>
-      <c r="C10" s="39" t="n">
+      <c r="C10" s="31" t="n">
         <v>54.576896615505</v>
       </c>
     </row>
@@ -41617,7 +41601,7 @@
       <c r="B11" s="38" t="n">
         <v>2.41</v>
       </c>
-      <c r="C11" s="39" t="n">
+      <c r="C11" s="31" t="n">
         <v>36.8432271269936</v>
       </c>
     </row>
@@ -41628,7 +41612,7 @@
       <c r="B12" s="38" t="n">
         <v>3.63</v>
       </c>
-      <c r="C12" s="39" t="n">
+      <c r="C12" s="31" t="n">
         <v>58.2688631512597</v>
       </c>
     </row>
@@ -41639,7 +41623,7 @@
       <c r="B13" s="38" t="n">
         <v>3.64</v>
       </c>
-      <c r="C13" s="39" t="n">
+      <c r="C13" s="31" t="n">
         <v>58.429383435423</v>
       </c>
     </row>
@@ -41650,7 +41634,7 @@
       <c r="B14" s="38" t="n">
         <v>3.86</v>
       </c>
-      <c r="C14" s="39" t="n">
+      <c r="C14" s="31" t="n">
         <v>65.221925986331</v>
       </c>
     </row>
@@ -41661,7 +41645,7 @@
       <c r="B15" s="38" t="n">
         <v>4.34</v>
       </c>
-      <c r="C15" s="39" t="n">
+      <c r="C15" s="31" t="n">
         <v>77.406448140945</v>
       </c>
     </row>
@@ -41672,7 +41656,7 @@
       <c r="B16" s="38" t="n">
         <v>3.64</v>
       </c>
-      <c r="C16" s="39" t="n">
+      <c r="C16" s="31" t="n">
         <v>64.92153715047</v>
       </c>
     </row>
@@ -41683,7 +41667,7 @@
       <c r="B17" s="38" t="n">
         <v>1.83</v>
       </c>
-      <c r="C17" s="39" t="n">
+      <c r="C17" s="31" t="n">
         <v>32.6391244465275</v>
       </c>
     </row>
@@ -41694,7 +41678,7 @@
       <c r="B18" s="38" t="n">
         <v>1.17</v>
       </c>
-      <c r="C18" s="39" t="n">
+      <c r="C18" s="31" t="n">
         <v>22.0951449965885</v>
       </c>
     </row>
@@ -41705,7 +41689,7 @@
       <c r="B19" s="38" t="n">
         <v>1.35</v>
       </c>
-      <c r="C19" s="39" t="n">
+      <c r="C19" s="31" t="n">
         <v>26.26695559035</v>
       </c>
     </row>
@@ -41716,7 +41700,7 @@
       <c r="B20" s="38" t="n">
         <v>2.56</v>
       </c>
-      <c r="C20" s="39" t="n">
+      <c r="C20" s="31" t="n">
         <v>51.36649093224</v>
       </c>
     </row>
@@ -41727,7 +41711,7 @@
       <c r="B21" s="38" t="n">
         <v>2.42</v>
       </c>
-      <c r="C21" s="39" t="n">
+      <c r="C21" s="31" t="n">
         <v>48.5573859593831</v>
       </c>
     </row>
@@ -41738,7 +41722,7 @@
       <c r="B22" s="38" t="n">
         <v>1.19</v>
       </c>
-      <c r="C22" s="39" t="n">
+      <c r="C22" s="31" t="n">
         <v>26.3474673316231</v>
       </c>
     </row>
@@ -41749,7 +41733,7 @@
       <c r="B23" s="38" t="n">
         <v>0.86</v>
       </c>
-      <c r="C23" s="39" t="n">
+      <c r="C23" s="31" t="n">
         <v>19.7210634829136</v>
       </c>
     </row>
@@ -41760,7 +41744,7 @@
       <c r="B24" s="38" t="n">
         <v>0.95</v>
       </c>
-      <c r="C24" s="39" t="n">
+      <c r="C24" s="31" t="n">
         <v>21.0336924075983</v>
       </c>
     </row>
@@ -41771,7 +41755,7 @@
       <c r="B25" s="38" t="n">
         <v>0.86</v>
       </c>
-      <c r="C25" s="39" t="n">
+      <c r="C25" s="31" t="n">
         <v>19.041026811089</v>
       </c>
     </row>
@@ -41782,7 +41766,7 @@
       <c r="B26" s="38" t="n">
         <v>0.78</v>
       </c>
-      <c r="C26" s="39" t="n">
+      <c r="C26" s="31" t="n">
         <v>17.2697685030807</v>
       </c>
     </row>
@@ -41793,7 +41777,7 @@
       <c r="B27" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="C27" s="39" t="n">
+      <c r="C27" s="31" t="n">
         <v>22.9314691661786</v>
       </c>
     </row>
@@ -41804,7 +41788,7 @@
       <c r="B28" s="38" t="n">
         <v>0.84</v>
       </c>
-      <c r="C28" s="39" t="n">
+      <c r="C28" s="31" t="n">
         <v>19.97585758476</v>
       </c>
     </row>
@@ -41815,7 +41799,7 @@
       <c r="B29" s="38" t="n">
         <v>0.88</v>
       </c>
-      <c r="C29" s="39" t="n">
+      <c r="C29" s="31" t="n">
         <v>20.92708889832</v>
       </c>
     </row>
@@ -41826,7 +41810,7 @@
       <c r="B30" s="38" t="n">
         <v>0.71</v>
       </c>
-      <c r="C30" s="39" t="n">
+      <c r="C30" s="31" t="n">
         <v>16.88435581569</v>
       </c>
     </row>
@@ -41837,7 +41821,7 @@
       <c r="B31" s="38" t="n">
         <v>0.67</v>
       </c>
-      <c r="C31" s="39" t="n">
+      <c r="C31" s="31" t="n">
         <v>15.93312450213</v>
       </c>
     </row>
@@ -41848,7 +41832,7 @@
       <c r="B32" s="38" t="n">
         <v>0.88</v>
       </c>
-      <c r="C32" s="39" t="n">
+      <c r="C32" s="31" t="n">
         <v>20.92708889832</v>
       </c>
     </row>
@@ -41859,7 +41843,7 @@
       <c r="B33" s="38" t="n">
         <v>0.94</v>
       </c>
-      <c r="C33" s="39" t="n">
+      <c r="C33" s="31" t="n">
         <v>22.35393586866</v>
       </c>
     </row>
@@ -41870,7 +41854,7 @@
       <c r="B34" s="38" t="n">
         <v>0.87</v>
       </c>
-      <c r="C34" s="39" t="n">
+      <c r="C34" s="31" t="n">
         <v>20.68928106993</v>
       </c>
     </row>
@@ -41881,7 +41865,7 @@
       <c r="B35" s="38" t="n">
         <v>0.67</v>
       </c>
-      <c r="C35" s="39" t="n">
+      <c r="C35" s="31" t="n">
         <v>15.93312450213</v>
       </c>
     </row>
@@ -41892,7 +41876,7 @@
       <c r="B36" s="38" t="n">
         <v>0.56</v>
       </c>
-      <c r="C36" s="39" t="n">
+      <c r="C36" s="31" t="n">
         <v>13.31723838984</v>
       </c>
     </row>
@@ -41903,7 +41887,7 @@
       <c r="B37" s="38" t="n">
         <v>0.64</v>
       </c>
-      <c r="C37" s="39" t="n">
+      <c r="C37" s="31" t="n">
         <v>15.21970101696</v>
       </c>
     </row>
@@ -41914,7 +41898,7 @@
       <c r="B38" s="38" t="n">
         <v>0.84</v>
       </c>
-      <c r="C38" s="39" t="n">
+      <c r="C38" s="31" t="n">
         <v>20.7441597995585</v>
       </c>
     </row>
@@ -41925,7 +41909,7 @@
       <c r="B39" s="38" t="n">
         <v>1.36</v>
       </c>
-      <c r="C39" s="39" t="n">
+      <c r="C39" s="31" t="n">
         <v>34.9292138339232</v>
       </c>
     </row>
@@ -41936,7 +41920,7 @@
       <c r="B40" s="38" t="n">
         <v>1.18</v>
       </c>
-      <c r="C40" s="39" t="n">
+      <c r="C40" s="31" t="n">
         <v>30.3062296500216</v>
       </c>
     </row>
@@ -41947,7 +41931,7 @@
       <c r="B41" s="38" t="n">
         <v>0.79</v>
       </c>
-      <c r="C41" s="39" t="n">
+      <c r="C41" s="31" t="n">
         <v>20.2897639182348</v>
       </c>
     </row>
@@ -41958,7 +41942,7 @@
       <c r="B42" s="38" t="n">
         <v>0.91</v>
       </c>
-      <c r="C42" s="39" t="n">
+      <c r="C42" s="31" t="n">
         <v>23.3717533741692</v>
       </c>
     </row>
@@ -41969,7 +41953,7 @@
       <c r="B43" s="38" t="n">
         <v>1.29</v>
       </c>
-      <c r="C43" s="39" t="n">
+      <c r="C43" s="31" t="n">
         <v>33.1313866512948</v>
       </c>
     </row>
@@ -41980,7 +41964,7 @@
       <c r="B44" s="38" t="n">
         <v>1.19</v>
       </c>
-      <c r="C44" s="39" t="n">
+      <c r="C44" s="31" t="n">
         <v>30.5630621046828</v>
       </c>
     </row>
@@ -41991,7 +41975,7 @@
       <c r="B45" s="38" t="n">
         <v>0.96</v>
       </c>
-      <c r="C45" s="39" t="n">
+      <c r="C45" s="31" t="n">
         <v>24.6559156474752</v>
       </c>
     </row>
@@ -42002,7 +41986,7 @@
       <c r="B46" s="38" t="n">
         <v>0.8</v>
       </c>
-      <c r="C46" s="39" t="n">
+      <c r="C46" s="31" t="n">
         <v>20.546596372896</v>
       </c>
     </row>
@@ -42013,7 +41997,7 @@
       <c r="B47" s="38" t="n">
         <v>0.94</v>
       </c>
-      <c r="C47" s="39" t="n">
+      <c r="C47" s="31" t="n">
         <v>23.2137026328392</v>
       </c>
     </row>
@@ -42024,7 +42008,7 @@
       <c r="B48" s="38" t="n">
         <v>0.86</v>
       </c>
-      <c r="C48" s="39" t="n">
+      <c r="C48" s="31" t="n">
         <v>20.45147324154</v>
       </c>
     </row>
@@ -42035,7 +42019,7 @@
       <c r="B49" s="38" t="n">
         <v>0.62</v>
       </c>
-      <c r="C49" s="39" t="n">
+      <c r="C49" s="31" t="n">
         <v>14.74408536018</v>
       </c>
     </row>
@@ -42046,7 +42030,7 @@
       <c r="B50" s="38" t="n">
         <v>0.73</v>
       </c>
-      <c r="C50" s="39" t="n">
+      <c r="C50" s="31" t="n">
         <v>17.35997147247</v>
       </c>
     </row>
@@ -42057,7 +42041,7 @@
       <c r="B51" s="38" t="n">
         <v>0.72</v>
       </c>
-      <c r="C51" s="39" t="n">
+      <c r="C51" s="31" t="n">
         <v>17.12216364408</v>
       </c>
     </row>
@@ -42068,7 +42052,7 @@
       <c r="B52" s="38" t="n">
         <v>0.72</v>
       </c>
-      <c r="C52" s="39" t="n">
+      <c r="C52" s="31" t="n">
         <v>16.5106577996486</v>
       </c>
     </row>
@@ -42079,7 +42063,7 @@
       <c r="B53" s="38" t="n">
         <v>0.7</v>
       </c>
-      <c r="C53" s="39" t="n">
+      <c r="C53" s="31" t="n">
         <v>16.6465479873</v>
       </c>
     </row>
@@ -42090,7 +42074,7 @@
       <c r="B54" s="38" t="n">
         <v>0.61</v>
       </c>
-      <c r="C54" s="39" t="n">
+      <c r="C54" s="31" t="n">
         <v>13.9881961913689</v>
       </c>
     </row>
@@ -42101,7 +42085,7 @@
       <c r="B55" s="38" t="n">
         <v>0.61</v>
       </c>
-      <c r="C55" s="39" t="n">
+      <c r="C55" s="31" t="n">
         <v>13.9881961913689</v>
       </c>
     </row>
@@ -42112,7 +42096,7 @@
       <c r="B56" s="38" t="n">
         <v>0.74</v>
       </c>
-      <c r="C56" s="39" t="n">
+      <c r="C56" s="31" t="n">
         <v>16.3841393490765</v>
       </c>
     </row>
@@ -42123,7 +42107,7 @@
       <c r="B57" s="38" t="n">
         <v>0.95</v>
       </c>
-      <c r="C57" s="39" t="n">
+      <c r="C57" s="31" t="n">
         <v>20.5379488155</v>
       </c>
     </row>
@@ -42134,7 +42118,7 @@
       <c r="B58" s="38" t="n">
         <v>0.81</v>
       </c>
-      <c r="C58" s="39" t="n">
+      <c r="C58" s="31" t="n">
         <v>17.2767075174</v>
       </c>
     </row>
@@ -42145,7 +42129,7 @@
       <c r="B59" s="38" t="n">
         <v>0.64</v>
       </c>
-      <c r="C59" s="39" t="n">
+      <c r="C59" s="31" t="n">
         <v>13.5148012224</v>
       </c>
     </row>
@@ -42156,7 +42140,7 @@
       <c r="B60" s="38" t="n">
         <v>1.1</v>
       </c>
-      <c r="C60" s="39" t="n">
+      <c r="C60" s="31" t="n">
         <v>21.597868864</v>
       </c>
     </row>
@@ -42167,7 +42151,7 @@
       <c r="B61" s="38" t="n">
         <v>1.56</v>
       </c>
-      <c r="C61" s="39" t="n">
+      <c r="C61" s="31" t="n">
         <v>26.0814347196</v>
       </c>
     </row>
@@ -42178,7 +42162,7 @@
       <c r="B62" s="38" t="n">
         <v>1.98</v>
       </c>
-      <c r="C62" s="39" t="n">
+      <c r="C62" s="31" t="n">
         <v>28.184369301</v>
       </c>
     </row>
@@ -42189,7 +42173,7 @@
       <c r="B63" s="38" t="n">
         <v>2.01</v>
       </c>
-      <c r="C63" s="39" t="n">
+      <c r="C63" s="31" t="n">
         <v>24.9201673923</v>
       </c>
     </row>
@@ -42200,7 +42184,7 @@
       <c r="B64" s="38" t="n">
         <v>3.07</v>
       </c>
-      <c r="C64" s="39" t="n">
+      <c r="C64" s="31" t="n">
         <v>32.8589803551</v>
       </c>
     </row>
@@ -42211,7 +42195,7 @@
       <c r="B65" s="38" t="n">
         <v>1.73</v>
       </c>
-      <c r="C65" s="39" t="n">
+      <c r="C65" s="31" t="n">
         <v>20.7286722085</v>
       </c>
     </row>
@@ -42222,7 +42206,7 @@
       <c r="B66" s="38" t="n">
         <v>1.61</v>
       </c>
-      <c r="C66" s="39" t="n">
+      <c r="C66" s="31" t="n">
         <v>20.5930204634</v>
       </c>
     </row>
@@ -42233,7 +42217,7 @@
       <c r="B67" s="38" t="n">
         <v>1.34</v>
       </c>
-      <c r="C67" s="39" t="n">
+      <c r="C67" s="31" t="n">
         <v>16.8376790006</v>
       </c>
     </row>
@@ -42244,7 +42228,7 @@
       <c r="B68" s="38" t="n">
         <v>1.43</v>
       </c>
-      <c r="C68" s="39" t="n">
+      <c r="C68" s="31" t="n">
         <v>17.9317533395</v>
       </c>
     </row>
@@ -42255,7 +42239,7 @@
       <c r="B69" s="38" t="n">
         <v>1.68</v>
       </c>
-      <c r="C69" s="39" t="n">
+      <c r="C69" s="31" t="n">
         <v>20.5476673416</v>
       </c>
     </row>
@@ -42266,7 +42250,7 @@
       <c r="B70" s="38" t="n">
         <v>1.88</v>
       </c>
-      <c r="C70" s="39" t="n">
+      <c r="C70" s="31" t="n">
         <v>22.7760202532</v>
       </c>
     </row>
@@ -42277,7 +42261,7 @@
       <c r="B71" s="38" t="n">
         <v>1.3</v>
       </c>
-      <c r="C71" s="39" t="n">
+      <c r="C71" s="31" t="n">
         <v>16.050585655</v>
       </c>
     </row>
@@ -42288,7 +42272,7 @@
       <c r="B72" s="38" t="n">
         <v>1.17</v>
       </c>
-      <c r="C72" s="39" t="n">
+      <c r="C72" s="31" t="n">
         <v>14.6413135557</v>
       </c>
     </row>
@@ -42299,7 +42283,7 @@
       <c r="B73" s="38" t="n">
         <v>1.27</v>
       </c>
-      <c r="C73" s="39" t="n">
+      <c r="C73" s="31" t="n">
         <v>15.8927078767</v>
       </c>
     </row>
@@ -42310,7 +42294,7 @@
       <c r="B74" s="38" t="n">
         <v>1.19</v>
       </c>
-      <c r="C74" s="39" t="n">
+      <c r="C74" s="31" t="n">
         <v>15.2821999358</v>
       </c>
     </row>
@@ -42321,7 +42305,7 @@
       <c r="B75" s="38" t="n">
         <v>0.65</v>
       </c>
-      <c r="C75" s="39" t="n">
+      <c r="C75" s="31" t="n">
         <v>9.1520411515</v>
       </c>
     </row>
@@ -42332,7 +42316,7 @@
       <c r="B76" s="38" t="n">
         <v>0.87</v>
       </c>
-      <c r="C76" s="39" t="n">
+      <c r="C76" s="31" t="n">
         <v>13.6569748923</v>
       </c>
     </row>
@@ -42343,7 +42327,7 @@
       <c r="B77" s="38" t="n">
         <v>0.67</v>
       </c>
-      <c r="C77" s="39" t="n">
+      <c r="C77" s="31" t="n">
         <v>11.0852126048</v>
       </c>
     </row>
@@ -42354,7 +42338,7 @@
       <c r="B78" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="C78" s="39" t="n">
+      <c r="C78" s="31" t="n">
         <v>16.01304168</v>
       </c>
     </row>
@@ -42365,7 +42349,7 @@
       <c r="B79" s="38" t="n">
         <v>0.97</v>
       </c>
-      <c r="C79" s="39" t="n">
+      <c r="C79" s="31" t="n">
         <v>15.1518258009</v>
       </c>
     </row>
@@ -42376,7 +42360,7 @@
       <c r="B80" s="38" t="n">
         <v>1.09</v>
       </c>
-      <c r="C80" s="39" t="n">
+      <c r="C80" s="31" t="n">
         <v>16.8672636529</v>
       </c>
     </row>
@@ -42387,7 +42371,7 @@
       <c r="B81" s="38" t="n">
         <v>1.18</v>
       </c>
-      <c r="C81" s="39" t="n">
+      <c r="C81" s="31" t="n">
         <v>17.6220262726</v>
       </c>
     </row>
@@ -42398,7 +42382,7 @@
       <c r="B82" s="38" t="n">
         <v>1.13</v>
       </c>
-      <c r="C82" s="39" t="n">
+      <c r="C82" s="31" t="n">
         <v>17.1953336333</v>
       </c>
     </row>
@@ -42409,7 +42393,7 @@
       <c r="B83" s="38" t="n">
         <v>1.02</v>
       </c>
-      <c r="C83" s="39" t="n">
+      <c r="C83" s="31" t="n">
         <v>15.744655893</v>
       </c>
     </row>
@@ -42420,7 +42404,7 @@
       <c r="B84" s="38" t="n">
         <v>1.02</v>
       </c>
-      <c r="C84" s="39" t="n">
+      <c r="C84" s="31" t="n">
         <v>15.5936647524</v>
       </c>
     </row>
@@ -42431,7 +42415,7 @@
       <c r="B85" s="38" t="n">
         <v>1.14</v>
       </c>
-      <c r="C85" s="39" t="n">
+      <c r="C85" s="31" t="n">
         <v>16.6015595784</v>
       </c>
     </row>
@@ -42442,7 +42426,7 @@
       <c r="B86" s="38" t="n">
         <v>1.19</v>
       </c>
-      <c r="C86" s="39" t="n">
+      <c r="C86" s="31" t="n">
         <v>15.6549365196</v>
       </c>
     </row>
@@ -42453,7 +42437,7 @@
       <c r="B87" s="38" t="n">
         <v>1.2</v>
       </c>
-      <c r="C87" s="39" t="n">
+      <c r="C87" s="31" t="n">
         <v>14.877711876</v>
       </c>
     </row>
@@ -42464,7 +42448,7 @@
       <c r="B88" s="38" t="n">
         <v>1.21</v>
       </c>
-      <c r="C88" s="39" t="n">
+      <c r="C88" s="31" t="n">
         <v>14.744698936</v>
       </c>
     </row>
@@ -42475,7 +42459,7 @@
       <c r="B89" s="38" t="n">
         <v>1.05</v>
       </c>
-      <c r="C89" s="39" t="n">
+      <c r="C89" s="31" t="n">
         <v>12.506648952</v>
       </c>
     </row>
@@ -42486,7 +42470,7 @@
       <c r="B90" s="38" t="n">
         <v>1.12</v>
       </c>
-      <c r="C90" s="39" t="n">
+      <c r="C90" s="31" t="n">
         <v>12.290395656</v>
       </c>
     </row>
@@ -42497,7 +42481,7 @@
       <c r="B91" s="38" t="n">
         <v>1.9</v>
       </c>
-      <c r="C91" s="39" t="n">
+      <c r="C91" s="31" t="n">
         <v>18.236932222</v>
       </c>
     </row>
@@ -42508,7 +42492,7 @@
       <c r="B92" s="38" t="n">
         <v>1.99</v>
       </c>
-      <c r="C92" s="39" t="n">
+      <c r="C92" s="31" t="n">
         <v>17.7218074313</v>
       </c>
     </row>
@@ -42519,7 +42503,7 @@
       <c r="B93" s="38" t="n">
         <v>1.78</v>
       </c>
-      <c r="C93" s="39" t="n">
+      <c r="C93" s="31" t="n">
         <v>16.0120548098</v>
       </c>
     </row>
@@ -42530,7 +42514,7 @@
       <c r="B94" s="38" t="n">
         <v>1.71</v>
       </c>
-      <c r="C94" s="39" t="n">
+      <c r="C94" s="31" t="n">
         <v>15.2282867877</v>
       </c>
     </row>
@@ -42541,7 +42525,7 @@
       <c r="B95" s="38" t="n">
         <v>1.71</v>
       </c>
-      <c r="C95" s="39" t="n">
+      <c r="C95" s="31" t="n">
         <v>14.1093690642</v>
       </c>
     </row>
@@ -42552,7 +42536,7 @@
       <c r="B96" s="38" t="n">
         <v>1.71</v>
       </c>
-      <c r="C96" s="39" t="n">
+      <c r="C96" s="31" t="n">
         <v>13.8122138655</v>
       </c>
     </row>
@@ -42563,7 +42547,7 @@
       <c r="B97" s="38" t="n">
         <v>1.93</v>
       </c>
-      <c r="C97" s="39" t="n">
+      <c r="C97" s="31" t="n">
         <v>15.4650069135</v>
       </c>
     </row>
@@ -42574,7 +42558,7 @@
       <c r="B98" s="38" t="n">
         <v>1.93</v>
       </c>
-      <c r="C98" s="39" t="n">
+      <c r="C98" s="31" t="n">
         <v>15.3904767597</v>
       </c>
     </row>
@@ -42585,7 +42569,7 @@
       <c r="B99" s="38" t="n">
         <v>1.93</v>
       </c>
-      <c r="C99" s="39" t="n">
+      <c r="C99" s="31" t="n">
         <v>15.4525852212</v>
       </c>
     </row>
@@ -42596,7 +42580,7 @@
       <c r="B100" s="38" t="n">
         <v>1.93</v>
       </c>
-      <c r="C100" s="39" t="n">
+      <c r="C100" s="31" t="n">
         <v>15.2289947598</v>
       </c>
     </row>
@@ -42607,7 +42591,7 @@
       <c r="B101" s="38" t="n">
         <v>1.9</v>
       </c>
-      <c r="C101" s="39" t="n">
+      <c r="C101" s="31" t="n">
         <v>14.466444447</v>
       </c>
     </row>
@@ -42618,7 +42602,7 @@
       <c r="B102" s="38" t="n">
         <v>2.08</v>
       </c>
-      <c r="C102" s="39" t="n">
+      <c r="C102" s="31" t="n">
         <v>15.4264117072</v>
       </c>
     </row>
@@ -42629,7 +42613,7 @@
       <c r="B103" s="38" t="n">
         <v>2.08</v>
       </c>
-      <c r="C103" s="39" t="n">
+      <c r="C103" s="31" t="n">
         <v>15.2925406192</v>
       </c>
     </row>
@@ -42640,7 +42624,7 @@
       <c r="B104" s="38" t="n">
         <v>1.9</v>
       </c>
-      <c r="C104" s="39" t="n">
+      <c r="C104" s="31" t="n">
         <v>13.749032719</v>
       </c>
     </row>
@@ -42651,7 +42635,7 @@
       <c r="B105" s="38" t="n">
         <v>1.8</v>
       </c>
-      <c r="C105" s="39" t="n">
+      <c r="C105" s="31" t="n">
         <v>12.89796444</v>
       </c>
     </row>
@@ -42662,7 +42646,7 @@
       <c r="B106" s="38" t="n">
         <v>1.8</v>
       </c>
-      <c r="C106" s="39" t="n">
+      <c r="C106" s="31" t="n">
         <v>12.758944464</v>
       </c>
     </row>
@@ -42673,7 +42657,7 @@
       <c r="B107" s="38" t="n">
         <v>1.8</v>
       </c>
-      <c r="C107" s="39" t="n">
+      <c r="C107" s="31" t="n">
         <v>12.60833949</v>
       </c>
     </row>
@@ -42684,7 +42668,7 @@
       <c r="B108" s="38" t="n">
         <v>1.8</v>
       </c>
-      <c r="C108" s="39" t="n">
+      <c r="C108" s="31" t="n">
         <v>12.43456452</v>
       </c>
     </row>
@@ -42695,7 +42679,7 @@
       <c r="B109" s="38" t="n">
         <v>1.8</v>
       </c>
-      <c r="C109" s="39" t="n">
+      <c r="C109" s="31" t="n">
         <v>12.226034556</v>
       </c>
     </row>
@@ -42706,7 +42690,7 @@
       <c r="B110" s="38" t="n">
         <v>1.8</v>
       </c>
-      <c r="C110" s="39" t="n">
+      <c r="C110" s="31" t="n">
         <v>11.89393128</v>
       </c>
     </row>
@@ -42717,7 +42701,7 @@
       <c r="B111" s="38" t="n">
         <v>1.8</v>
       </c>
-      <c r="C111" s="39" t="n">
+      <c r="C111" s="31" t="n">
         <v>11.557966338</v>
       </c>
     </row>
@@ -42728,7 +42712,7 @@
       <c r="B112" s="38" t="n">
         <v>1.8</v>
       </c>
-      <c r="C112" s="39" t="n">
+      <c r="C112" s="31" t="n">
         <v>11.094566418</v>
       </c>
     </row>
@@ -42739,7 +42723,7 @@
       <c r="B113" s="38" t="n">
         <v>1.8</v>
       </c>
-      <c r="C113" s="39" t="n">
+      <c r="C113" s="31" t="n">
         <v>10.526901516</v>
       </c>
     </row>
@@ -42750,7 +42734,7 @@
       <c r="B114" s="38" t="n">
         <v>1.8</v>
       </c>
-      <c r="C114" s="39" t="n">
+      <c r="C114" s="31" t="n">
         <v>9.939928284</v>
       </c>
     </row>
@@ -42761,7 +42745,7 @@
       <c r="B115" s="38" t="n">
         <v>2.24</v>
       </c>
-      <c r="C115" s="39" t="n">
+      <c r="C115" s="31" t="n">
         <v>11.8506806208</v>
       </c>
     </row>
@@ -42772,7 +42756,7 @@
       <c r="B116" s="38" t="n">
         <v>2.48</v>
       </c>
-      <c r="C116" s="39" t="n">
+      <c r="C116" s="31" t="n">
         <v>12.7213575816</v>
       </c>
     </row>
@@ -42783,7 +42767,7 @@
       <c r="B117" s="38" t="n">
         <v>3.29</v>
       </c>
-      <c r="C117" s="39" t="n">
+      <c r="C117" s="31" t="n">
         <v>15.8881596923</v>
       </c>
     </row>
@@ -42794,7 +42778,7 @@
       <c r="B118" s="38" t="n">
         <v>11.58</v>
       </c>
-      <c r="C118" s="39" t="n">
+      <c r="C118" s="31" t="n">
         <v>50.4072273534</v>
       </c>
     </row>
@@ -42805,7 +42789,7 @@
       <c r="B119" s="38" t="n">
         <v>11.53</v>
       </c>
-      <c r="C119" s="39" t="n">
+      <c r="C119" s="31" t="n">
         <v>45.9844398299</v>
       </c>
     </row>
@@ -42816,7 +42800,7 @@
       <c r="B120" s="38" t="n">
         <v>12.8</v>
       </c>
-      <c r="C120" s="39" t="n">
+      <c r="C120" s="31" t="n">
         <v>48.248513152</v>
       </c>
     </row>
@@ -42827,7 +42811,7 @@
       <c r="B121" s="38" t="n">
         <v>13.92</v>
       </c>
-      <c r="C121" s="39" t="n">
+      <c r="C121" s="31" t="n">
         <v>49.2449946096</v>
       </c>
     </row>
@@ -42838,7 +42822,7 @@
       <c r="B122" s="38" t="n">
         <v>14.02</v>
       </c>
-      <c r="C122" s="39" t="n">
+      <c r="C122" s="31" t="n">
         <v>46.1320358895706</v>
       </c>
     </row>
@@ -42849,7 +42833,7 @@
       <c r="B123" s="38" t="n">
         <v>31.61</v>
       </c>
-      <c r="C123" s="39" t="n">
+      <c r="C123" s="31" t="n">
         <v>93.4092915977962</v>
       </c>
     </row>
@@ -42860,7 +42844,7 @@
       <c r="B124" s="38" t="n">
         <v>36.83</v>
       </c>
-      <c r="C124" s="39" t="n">
+      <c r="C124" s="31" t="n">
         <v>95.890748907767</v>
       </c>
     </row>
@@ -42871,7 +42855,7 @@
       <c r="B125" s="38" t="n">
         <v>35.93</v>
       </c>
-      <c r="C125" s="39" t="n">
+      <c r="C125" s="31" t="n">
         <v>84.7999385038504</v>
       </c>
     </row>
@@ -42882,7 +42866,7 @@
       <c r="B126" s="38" t="n">
         <v>32.97</v>
       </c>
-      <c r="C126" s="39" t="n">
+      <c r="C126" s="31" t="n">
         <v>73.298289015544</v>
       </c>
     </row>
@@ -42893,7 +42877,7 @@
       <c r="B127" s="38" t="n">
         <v>29.55</v>
       </c>
-      <c r="C127" s="39" t="n">
+      <c r="C127" s="31" t="n">
         <v>63.6502846385542</v>
       </c>
     </row>
@@ -42904,7 +42888,7 @@
       <c r="B128" s="38" t="n">
         <v>28.78</v>
       </c>
-      <c r="C128" s="39" t="n">
+      <c r="C128" s="31" t="n">
         <v>59.426129547642</v>
       </c>
     </row>
@@ -42915,7 +42899,7 @@
       <c r="B129" s="38" t="n">
         <v>27.56</v>
       </c>
-      <c r="C129" s="39" t="n">
+      <c r="C129" s="31" t="n">
         <v>54.9501832713755</v>
       </c>
     </row>
@@ -42926,7 +42910,7 @@
       <c r="B130" s="38" t="n">
         <v>14.43</v>
       </c>
-      <c r="C130" s="39" t="n">
+      <c r="C130" s="31" t="n">
         <v>28.2460666970803</v>
       </c>
     </row>
@@ -42937,7 +42921,7 @@
       <c r="B131" s="31" t="n">
         <v>18.4350394</v>
       </c>
-      <c r="C131" s="39" t="n">
+      <c r="C131" s="31" t="n">
         <v>34.8151236598398</v>
       </c>
     </row>
@@ -42948,7 +42932,7 @@
       <c r="B132" s="31" t="n">
         <v>14.9238417</v>
       </c>
-      <c r="C132" s="39" t="n">
+      <c r="C132" s="31" t="n">
         <v>27.0643806153246</v>
       </c>
     </row>
@@ -42959,7 +42943,7 @@
       <c r="B133" s="31" t="n">
         <v>18.2261133</v>
       </c>
-      <c r="C133" s="39" t="n">
+      <c r="C133" s="31" t="n">
         <v>31.5336747503395</v>
       </c>
     </row>
@@ -42970,7 +42954,7 @@
       <c r="B134" s="31" t="n">
         <v>23.7258203</v>
       </c>
-      <c r="C134" s="39" t="n">
+      <c r="C134" s="31" t="n">
         <v>38.9446542440788</v>
       </c>
     </row>
@@ -42981,7 +42965,7 @@
       <c r="B135" s="31" t="n">
         <v>20.0033852</v>
       </c>
-      <c r="C135" s="39" t="n">
+      <c r="C135" s="31" t="n">
         <v>31.5085627801204</v>
       </c>
     </row>
@@ -42992,7 +42976,7 @@
       <c r="B136" s="31" t="n">
         <v>19.3208366</v>
       </c>
-      <c r="C136" s="39" t="n">
+      <c r="C136" s="31" t="n">
         <v>29.5440792705217</v>
       </c>
     </row>
@@ -43003,7 +42987,7 @@
       <c r="B137" s="31" t="n">
         <v>16.9716342</v>
       </c>
-      <c r="C137" s="39" t="n">
+      <c r="C137" s="31" t="n">
         <v>25.1975327776152</v>
       </c>
     </row>
@@ -43014,7 +42998,7 @@
       <c r="B138" s="31" t="n">
         <v>15.8173152</v>
       </c>
-      <c r="C138" s="39" t="n">
+      <c r="C138" s="31" t="n">
         <v>22.8974315186397</v>
       </c>
     </row>
@@ -43025,7 +43009,7 @@
       <c r="B139" s="31" t="n">
         <v>17.0166797</v>
       </c>
-      <c r="C139" s="39" t="n">
+      <c r="C139" s="31" t="n">
         <v>23.9547730498615</v>
       </c>
     </row>
@@ -43036,7 +43020,7 @@
       <c r="B140" s="31" t="n">
         <v>20.6684884</v>
       </c>
-      <c r="C140" s="39" t="n">
+      <c r="C140" s="31" t="n">
         <v>28.2610292917196</v>
       </c>
     </row>
@@ -43047,7 +43031,7 @@
       <c r="B141" s="31" t="n">
         <v>19.0925875</v>
       </c>
-      <c r="C141" s="39" t="n">
+      <c r="C141" s="31" t="n">
         <v>25.5206632055296</v>
       </c>
     </row>
@@ -43058,7 +43042,7 @@
       <c r="B142" s="31" t="n">
         <v>12.7156615</v>
       </c>
-      <c r="C142" s="39" t="n">
+      <c r="C142" s="31" t="n">
         <v>16.7360728296043</v>
       </c>
     </row>
@@ -43069,7 +43053,7 @@
       <c r="B143" s="31" t="n">
         <v>17.9700778</v>
       </c>
-      <c r="C143" s="39" t="n">
+      <c r="C143" s="31" t="n">
         <v>23.1407357801837</v>
       </c>
     </row>
@@ -43080,7 +43064,7 @@
       <c r="B144" s="31" t="n">
         <v>28.4954492</v>
       </c>
-      <c r="C144" s="39" t="n">
+      <c r="C144" s="31" t="n">
         <v>35.5013251162625</v>
       </c>
     </row>
@@ -43091,7 +43075,7 @@
       <c r="B145" s="31" t="n">
         <v>24.4438911</v>
       </c>
-      <c r="C145" s="39" t="n">
+      <c r="C145" s="31" t="n">
         <v>29.611061913725</v>
       </c>
     </row>
@@ -43102,7 +43086,7 @@
       <c r="B146" s="31" t="n">
         <v>25.0232558</v>
       </c>
-      <c r="C146" s="39" t="n">
+      <c r="C146" s="31" t="n">
         <v>29.8411018875186</v>
       </c>
     </row>
@@ -43113,7 +43097,7 @@
       <c r="B147" s="31" t="n">
         <v>28.8307031</v>
       </c>
-      <c r="C147" s="39" t="n">
+      <c r="C147" s="31" t="n">
         <v>33.6155029943734</v>
       </c>
     </row>
@@ -43124,67 +43108,67 @@
       <c r="B148" s="31" t="n">
         <v>38.265</v>
       </c>
-      <c r="C148" s="39" t="n">
+      <c r="C148" s="31" t="n">
         <v>43.458222895712</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="40" t="n">
+      <c r="A149" s="34" t="n">
         <v>2005</v>
       </c>
       <c r="B149" s="31" t="n">
         <v>54.5210895</v>
       </c>
-      <c r="C149" s="41" t="n">
+      <c r="C149" s="35" t="n">
         <v>59.8914028574578</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="40" t="n">
+      <c r="A150" s="34" t="n">
         <v>2006</v>
       </c>
       <c r="B150" s="31" t="n">
         <v>65.1440625</v>
       </c>
-      <c r="C150" s="41" t="n">
+      <c r="C150" s="35" t="n">
         <v>69.3244629789807</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="40" t="n">
+      <c r="A151" s="34" t="n">
         <v>2007</v>
       </c>
       <c r="B151" s="31" t="n">
         <v>72.3890784</v>
       </c>
-      <c r="C151" s="41" t="n">
+      <c r="C151" s="35" t="n">
         <v>74.9010606278554</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="40" t="n">
+      <c r="A152" s="34" t="n">
         <v>2008</v>
       </c>
       <c r="B152" s="35" t="n">
         <v>97.2559728</v>
       </c>
-      <c r="C152" s="41" t="n">
+      <c r="C152" s="35" t="n">
         <v>96.909957764609</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="42" t="n">
+      <c r="A153" s="39" t="n">
         <v>2009</v>
       </c>
-      <c r="B153" s="43" t="n">
+      <c r="B153" s="40" t="n">
         <v>61.6712648</v>
       </c>
-      <c r="C153" s="44" t="n">
+      <c r="C153" s="40" t="n">
         <v>61.6712648</v>
       </c>
     </row>
     <row r="154" s="30" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="40"/>
+      <c r="A154" s="34"/>
       <c r="B154" s="35"/>
     </row>
     <row r="155" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43225,7 +43209,7 @@
   <dimension ref="A1:F710"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="1" sqref="D24 H13"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -48932,8 +48916,8 @@
   </sheetPr>
   <dimension ref="A3:C711"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="1" sqref="D24 I17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -48956,7 +48940,7 @@
       <c r="B4" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="45" t="n">
+      <c r="C4" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>
@@ -48968,7 +48952,7 @@
       <c r="B5" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="45" t="n">
+      <c r="C5" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>
@@ -48980,7 +48964,7 @@
       <c r="B6" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="45" t="n">
+      <c r="C6" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>
@@ -48992,7 +48976,7 @@
       <c r="B7" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="45" t="n">
+      <c r="C7" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>
@@ -49004,7 +48988,7 @@
       <c r="B8" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="45" t="n">
+      <c r="C8" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>
@@ -49016,7 +49000,7 @@
       <c r="B9" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="45" t="n">
+      <c r="C9" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>
@@ -49028,7 +49012,7 @@
       <c r="B10" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="45" t="n">
+      <c r="C10" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>
@@ -49040,7 +49024,7 @@
       <c r="B11" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="45" t="n">
+      <c r="C11" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>
@@ -49052,7 +49036,7 @@
       <c r="B12" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="45" t="n">
+      <c r="C12" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>
@@ -49064,7 +49048,7 @@
       <c r="B13" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="45" t="n">
+      <c r="C13" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>
@@ -49076,7 +49060,7 @@
       <c r="B14" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="45" t="n">
+      <c r="C14" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>
@@ -49088,7 +49072,7 @@
       <c r="B15" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="45" t="n">
+      <c r="C15" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>
@@ -49100,7 +49084,7 @@
       <c r="B16" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="45" t="n">
+      <c r="C16" s="41" t="n">
         <f aca="false">[4]Feuil1!$C$60/12</f>
         <v>0</v>
       </c>

</xml_diff>